<commit_message>
DMP real time added
</commit_message>
<xml_diff>
--- a/src/main/java/Mccm/Pega/TestData/PegaTestData.xlsx
+++ b/src/main/java/Mccm/Pega/TestData/PegaTestData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F66D67C2-FDAF-4E64-B2E4-2FD8545ACADD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prout21\git\Automation_Framework\MCCM\MCCM\src\main\java\Mccm\Pega\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC487CC-6F95-4FEF-A13F-2E0EAD0CA12B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15660" windowHeight="11820" xr2:uid="{FF52DB76-C817-42DB-890D-C15C61C74666}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{FF52DB76-C817-42DB-890D-C15C61C74666}"/>
   </bookViews>
   <sheets>
     <sheet name="PegaTestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>NBACampaignName</t>
   </si>
@@ -75,6 +79,12 @@
   </si>
   <si>
     <t>MCCM LC Outbound</t>
+  </si>
+  <si>
+    <t>DMPRealtimecontainers</t>
+  </si>
+  <si>
+    <t>CSM</t>
   </si>
 </sst>
 </file>
@@ -433,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F0B5D7-FA7D-4869-B85C-A65D364621F0}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,9 +460,10 @@
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -486,8 +497,11 @@
       <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -520,6 +534,9 @@
       </c>
       <c r="K2" t="s">
         <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle hard coded -API
</commit_message>
<xml_diff>
--- a/src/main/java/Mccm/Pega/TestData/PegaTestData.xlsx
+++ b/src/main/java/Mccm/Pega/TestData/PegaTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9C929EBE-A9D6-40A5-90D6-22702C7A011C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A8CEE460-F072-4BF8-BDB0-E81029E85BAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="15660" windowHeight="11820" xr2:uid="{FF52DB76-C817-42DB-890D-C15C61C74666}"/>
   </bookViews>
@@ -84,7 +84,7 @@
     <t>CSM</t>
   </si>
   <si>
-    <t>NBABatchCamptestc4</t>
+    <t>CampaignCD</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>